<commit_message>
"modificacion formato de planeacion"
</commit_message>
<xml_diff>
--- a/Documentos/FormatosPlaneacion/v2/individual/Formato de planeacion Alejandro.xlsx
+++ b/Documentos/FormatosPlaneacion/v2/individual/Formato de planeacion Alejandro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benkei\Desktop\SOFT2\ProyectoSoftwareII\Documentos\FormatosPlaneacion\v2\individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62659635-333C-46E0-BCBA-9FBDF175163C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF888E-4C8C-4843-9B3C-0C7FB3C993B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -846,7 +846,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1328,12 @@
       <c r="F27" s="19">
         <v>30</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="19">
+        <v>3</v>
+      </c>
       <c r="H27" s="18">
         <f t="shared" ref="H27:H28" si="7">IF(D27=G27,E27,0)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1352,10 +1354,12 @@
       <c r="F28" s="19">
         <v>100</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="19">
+        <v>3</v>
+      </c>
       <c r="H28" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,10 +1392,12 @@
       <c r="F30" s="19">
         <v>20</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="19">
+        <v>3</v>
+      </c>
       <c r="H30" s="18">
         <f t="shared" ref="H30:H31" si="9">IF(D30=G30,E30,0)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1451,7 +1457,7 @@
       <c r="G33" s="32"/>
       <c r="H33" s="34">
         <f>SUM(H14:H31)</f>
-        <v>0.72916666666666663</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Documentacion AsignarEnfermero y formato de planeacion
</commit_message>
<xml_diff>
--- a/Documentos/FormatosPlaneacion/v2/individual/Formato de planeacion Alejandro.xlsx
+++ b/Documentos/FormatosPlaneacion/v2/individual/Formato de planeacion Alejandro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benkei\Desktop\SOFT2\ProyectoSoftwareII\Documentos\FormatosPlaneacion\v2\individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF888E-4C8C-4843-9B3C-0C7FB3C993B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB15A8E9-9368-4319-ACEE-87FFE89E1DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1246,9 +1246,9 @@
       <c r="G23" s="23"/>
       <c r="H23" s="22"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="17">
@@ -1272,7 +1272,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="16" t="s">
         <v>29</v>
@@ -1310,7 +1310,7 @@
       <c r="G26" s="23"/>
       <c r="H26" s="22"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="16" t="s">
         <v>31</v>
@@ -1374,7 +1374,7 @@
       <c r="G29" s="23"/>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="16" t="s">
         <v>33</v>

</xml_diff>